<commit_message>
Test Extraction on Git ✨ 23 ธ.ค. 63 เวลา 16:40
</commit_message>
<xml_diff>
--- a/dataset/xlsx/covid-tracker.xlsx
+++ b/dataset/xlsx/covid-tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="156">
   <si>
     <t>status</t>
   </si>
@@ -124,6 +124,9 @@
     <t>2020-12-20</t>
   </si>
   <si>
+    <t>2020-12-22</t>
+  </si>
+  <si>
     <t>2020-12-23</t>
   </si>
   <si>
@@ -229,6 +232,9 @@
     <t>สำนักงานขนส่งเขตบางขุนเทียน</t>
   </si>
   <si>
+    <t>ตลาดหน้าสถานีรถไฟภาชี</t>
+  </si>
+  <si>
     <t>INC2 Tower B</t>
   </si>
   <si>
@@ -250,10 +256,19 @@
     <t>ตลาดหนองเสือ</t>
   </si>
   <si>
+    <t>ตลาดทะเลไทย</t>
+  </si>
+  <si>
+    <t>Lamptitude สาขาเอกมัย</t>
+  </si>
+  <si>
+    <t>กรมชลประทาน</t>
+  </si>
+  <si>
     <t>Siam Center</t>
   </si>
   <si>
-    <t>อาคารกรุงเทพประกันภัย</t>
+    <t>อาคารกรุงเทพประกันภัย ชั้น 22</t>
   </si>
   <si>
     <t>male</t>
@@ -364,6 +379,9 @@
     <t>เคสบุคลากร สวทช. ติดโควิด-19 ได้เข้ามาต่อใบขับขี่ที่นี่วันที่ 15 ธ.ค. ตรวจพบเชื้อตอนเย็นวันที่ 17 ธ.ค.</t>
   </si>
   <si>
+    <t>แม่ค้าอาหารทะเล ติดเชื้อจากการเดินทางไปตลาดทะเลไทย จ.สมุทรสาคร</t>
+  </si>
+  <si>
     <t>เคสบุคลากร สวทช. ติดโควิด-19 ได้เข้ามาปฏิบัติงานที่นี่วันที่ 16-17 ธ.ค. ตรวจพบเชื้อตอนเย็นวันที่ 17 ธ.ค.</t>
   </si>
   <si>
@@ -379,6 +397,15 @@
     <t>เจ้าของร้านอาหารที่ติดโควิดได้ไปขายเนื้อสดที่ตลาด</t>
   </si>
   <si>
+    <t>พบแม่ค้าอยุธยาเดินทางมาซื้ออาหารทะเลที่นี่และติดเชื่อโควิด-19</t>
+  </si>
+  <si>
+    <t>พนักงาน Lamptitude ติดเชื้อหลังจากกลับจากกระบี่ และเข้ามาที่นี่ตั้งแต่วันที่ 14-22 ธ.ค.</t>
+  </si>
+  <si>
+    <t>เจ้าหน้าที่กรมชลประทานพบผู้ติดเชื้อโควิด-19 เบื้องต้น 1 ราย เป็นวิศวกร สังกัด​กองพัฒนาแหล่ง​น้ำ​ขนาดกลาง โดยได้เดินทางไปรับประทานอาหารในพื้นที่เสี่ยง จังหวัดสมุทรสาคร เมื่อวันที่ 13 ธันวาคมที่ผ่านมา</t>
+  </si>
+  <si>
     <t>สยามเซ็นเตอร์' ประกาศยืนยันมี พนง.ร้านอาหารติดเชื้อโควิด-19 ขอปิดบริการพื้นที่เสี่ยง 3 วัน</t>
   </si>
   <si>
@@ -427,6 +454,9 @@
     <t>https://www.thairath.co.th/news/local/central/1999153</t>
   </si>
   <si>
+    <t>https://www.thairath.co.th/news/local/central/1999848</t>
+  </si>
+  <si>
     <t>https://www.thaipost.net/main/detail/87367</t>
   </si>
   <si>
@@ -440,6 +470,12 @@
   </si>
   <si>
     <t>https://www.thairath.co.th/news/local/central/1998795?cx_testId=0&amp;cx_testVariant=cx_0&amp;cx_artPos=0&amp;cx_rec_section=news&amp;cx_rec_topic=local#cxrecs_s</t>
+  </si>
+  <si>
+    <t>https://www.pptvhd36.com/news/%E0%B8%AA%E0%B8%B1%E0%B8%87%E0%B8%84%E0%B8%A1/138884</t>
+  </si>
+  <si>
+    <t>https://www.prachachat.net/economy/news-579476</t>
   </si>
   <si>
     <t>https://ch3thailandnews.bectero.com/news/224324</t>
@@ -816,7 +852,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -871,7 +907,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <v>12.674583</v>
@@ -892,13 +928,13 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -912,7 +948,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3">
         <v>13.7250712</v>
@@ -933,13 +969,13 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -953,7 +989,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>12.6838253</v>
@@ -974,13 +1010,13 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="M4">
         <v>2</v>
@@ -994,7 +1030,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5">
         <v>12.6959971</v>
@@ -1015,13 +1051,13 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K5" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="M5">
         <v>3</v>
@@ -1035,7 +1071,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D6">
         <v>12.6833042</v>
@@ -1056,13 +1092,13 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K6" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="M6">
         <v>4</v>
@@ -1076,7 +1112,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>13.653942</v>
@@ -1088,22 +1124,22 @@
         <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H7" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K7" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="M7">
         <v>5</v>
@@ -1117,7 +1153,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D8">
         <v>13.700916</v>
@@ -1129,22 +1165,22 @@
         <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H8" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K8" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="M8">
         <v>6</v>
@@ -1158,7 +1194,7 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9">
         <v>13.829441</v>
@@ -1170,22 +1206,22 @@
         <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H9" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J9" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K9" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="M9">
         <v>7</v>
@@ -1199,7 +1235,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D10">
         <v>13.759791</v>
@@ -1211,22 +1247,22 @@
         <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H10" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I10" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J10" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K10" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="M10">
         <v>8</v>
@@ -1240,7 +1276,7 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D11">
         <v>13.845817</v>
@@ -1252,22 +1288,22 @@
         <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I11" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J11" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K11" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="M11">
         <v>9</v>
@@ -1281,7 +1317,7 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12">
         <v>18.81089258</v>
@@ -1293,22 +1329,22 @@
         <v>29</v>
       </c>
       <c r="G12" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K12" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="M12">
         <v>10</v>
@@ -1322,7 +1358,7 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13">
         <v>18.80951974</v>
@@ -1334,22 +1370,22 @@
         <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H13" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J13" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K13" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="M13">
         <v>11</v>
@@ -1363,7 +1399,7 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D14">
         <v>18.80401814</v>
@@ -1375,22 +1411,22 @@
         <v>29</v>
       </c>
       <c r="G14" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H14" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J14" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K14" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="M14">
         <v>12</v>
@@ -1404,7 +1440,7 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15">
         <v>18.80732484</v>
@@ -1416,22 +1452,22 @@
         <v>29</v>
       </c>
       <c r="G15" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H15" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I15" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J15" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K15" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="M15">
         <v>13</v>
@@ -1445,7 +1481,7 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D16">
         <v>18.80709567</v>
@@ -1457,22 +1493,22 @@
         <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H16" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J16" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K16" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="M16">
         <v>14</v>
@@ -1486,7 +1522,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D17">
         <v>18.80650918</v>
@@ -1498,22 +1534,22 @@
         <v>29</v>
       </c>
       <c r="G17" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H17" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I17" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J17" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K17" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="M17">
         <v>15</v>
@@ -1527,7 +1563,7 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18">
         <v>18.80657601</v>
@@ -1539,22 +1575,22 @@
         <v>29</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H18" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I18" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J18" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K18" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="M18">
         <v>16</v>
@@ -1568,7 +1604,7 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D19">
         <v>18.80658294</v>
@@ -1580,22 +1616,22 @@
         <v>29</v>
       </c>
       <c r="G19" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H19" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J19" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K19" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="M19">
         <v>17</v>
@@ -1609,7 +1645,7 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20">
         <v>18.80675924</v>
@@ -1621,22 +1657,22 @@
         <v>29</v>
       </c>
       <c r="G20" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H20" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J20" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K20" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="M20">
         <v>18</v>
@@ -1650,7 +1686,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D21">
         <v>18.80629446</v>
@@ -1662,22 +1698,22 @@
         <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H21" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J21" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K21" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="M21">
         <v>19</v>
@@ -1691,7 +1727,7 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D22">
         <v>19.85327262</v>
@@ -1703,22 +1739,22 @@
         <v>28</v>
       </c>
       <c r="G22" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H22" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I22" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J22" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K22" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="M22">
         <v>20</v>
@@ -1732,7 +1768,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D23">
         <v>19.90661769</v>
@@ -1744,22 +1780,22 @@
         <v>28</v>
       </c>
       <c r="G23" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H23" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I23" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J23" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K23" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="M23">
         <v>21</v>
@@ -1773,7 +1809,7 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D24">
         <v>19.6476693</v>
@@ -1785,22 +1821,22 @@
         <v>28</v>
       </c>
       <c r="G24" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H24" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I24" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J24" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K24" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="M24">
         <v>22</v>
@@ -1814,7 +1850,7 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>13.7238495</v>
@@ -1826,22 +1862,22 @@
         <v>26</v>
       </c>
       <c r="G25" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H25" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J25" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K25" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="M25">
         <v>23</v>
@@ -1855,7 +1891,7 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D26">
         <v>13.7285268</v>
@@ -1867,22 +1903,22 @@
         <v>26</v>
       </c>
       <c r="G26" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H26" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I26" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J26" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K26" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="M26">
         <v>24</v>
@@ -1896,7 +1932,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D27">
         <v>13.7292718</v>
@@ -1908,22 +1944,22 @@
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H27" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I27" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J27" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K27" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="M27">
         <v>25</v>
@@ -1937,7 +1973,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D28">
         <v>14.896466</v>
@@ -1949,22 +1985,22 @@
         <v>51</v>
       </c>
       <c r="G28" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H28" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I28" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J28" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K28" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="M28">
         <v>26</v>
@@ -1978,7 +2014,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D29">
         <v>13.7499881</v>
@@ -1999,13 +2035,13 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K29" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="M29">
         <v>27</v>
@@ -2019,7 +2055,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D30">
         <v>13.6910012</v>
@@ -2040,13 +2076,13 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K30" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="M30">
         <v>28</v>
@@ -2060,7 +2096,7 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D31">
         <v>13.7468252</v>
@@ -2081,13 +2117,13 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K31" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="M31">
         <v>29</v>
@@ -2101,7 +2137,7 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D32">
         <v>13.7449539</v>
@@ -2122,13 +2158,13 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K32" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="M32">
         <v>30</v>
@@ -2142,7 +2178,7 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D33">
         <v>13.8205741</v>
@@ -2163,13 +2199,13 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K33" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="M33">
         <v>31</v>
@@ -2183,7 +2219,7 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D34">
         <v>13.5455607</v>
@@ -2204,13 +2240,13 @@
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K34" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="M34">
         <v>32</v>
@@ -2224,7 +2260,7 @@
         <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D35">
         <v>13.5440411</v>
@@ -2245,13 +2281,13 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K35" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="M35">
         <v>33</v>
@@ -2265,7 +2301,7 @@
         <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D36">
         <v>13.6211105</v>
@@ -2286,13 +2322,13 @@
         <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K36" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="M36">
         <v>34</v>
@@ -2306,7 +2342,7 @@
         <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D37">
         <v>13.8330877</v>
@@ -2327,13 +2363,13 @@
         <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K37" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="M37">
         <v>35</v>
@@ -2344,16 +2380,16 @@
         <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D38">
-        <v>14.0782451</v>
+        <v>14.45160513</v>
       </c>
       <c r="E38">
-        <v>100.604118</v>
+        <v>100.7230585</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -2368,13 +2404,13 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K38" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="M38">
         <v>36</v>
@@ -2382,19 +2418,19 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D39">
-        <v>13.5579068</v>
+        <v>14.0782451</v>
       </c>
       <c r="E39">
-        <v>100.270829</v>
+        <v>100.604118</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2409,13 +2445,13 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K39" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="M39">
         <v>37</v>
@@ -2423,25 +2459,25 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D40">
-        <v>14.1487352</v>
+        <v>13.5579068</v>
       </c>
       <c r="E40">
-        <v>100.6155778</v>
+        <v>100.270829</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
-      <c r="G40" t="s">
-        <v>81</v>
+      <c r="G40">
+        <v>0</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -2450,13 +2486,13 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K40" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="M40">
         <v>38</v>
@@ -2464,25 +2500,25 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
         <v>34</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D41">
-        <v>13.8057625</v>
+        <v>14.1487352</v>
       </c>
       <c r="E41">
-        <v>100.6621959</v>
+        <v>100.6155778</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
-      <c r="G41">
-        <v>0</v>
+      <c r="G41" t="s">
+        <v>86</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -2491,13 +2527,13 @@
         <v>0</v>
       </c>
       <c r="J41" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K41" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="M41">
         <v>39</v>
@@ -2508,16 +2544,16 @@
         <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D42">
-        <v>13.7937004</v>
+        <v>13.8057625</v>
       </c>
       <c r="E42">
-        <v>100.6923144</v>
+        <v>100.6621959</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2532,13 +2568,13 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K42" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="M42">
         <v>40</v>
@@ -2546,19 +2582,19 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D43">
-        <v>13.7204469</v>
+        <v>13.7937004</v>
       </c>
       <c r="E43">
-        <v>100.5004708</v>
+        <v>100.6923144</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -2573,13 +2609,13 @@
         <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K43" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="M43">
         <v>41</v>
@@ -2587,19 +2623,19 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B44" t="s">
         <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D44">
-        <v>14.3355326</v>
+        <v>13.7204469</v>
       </c>
       <c r="E44">
-        <v>100.87017</v>
+        <v>100.5004708</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -2614,13 +2650,13 @@
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="M44">
         <v>42</v>
@@ -2634,13 +2670,13 @@
         <v>35</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D45">
-        <v>14.5786407</v>
+        <v>14.3355326</v>
       </c>
       <c r="E45">
-        <v>100.9662444</v>
+        <v>100.87017</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -2655,13 +2691,13 @@
         <v>0</v>
       </c>
       <c r="J45" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K45" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="M45">
         <v>43</v>
@@ -2675,13 +2711,13 @@
         <v>35</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D46">
-        <v>14.5116599</v>
+        <v>14.5786407</v>
       </c>
       <c r="E46">
-        <v>100.9094134</v>
+        <v>100.9662444</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -2696,13 +2732,13 @@
         <v>0</v>
       </c>
       <c r="J46" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K46" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="M46">
         <v>44</v>
@@ -2710,19 +2746,19 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
         <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D47">
-        <v>14.1378761</v>
+        <v>14.5116599</v>
       </c>
       <c r="E47">
-        <v>100.8255049</v>
+        <v>100.9094134</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -2737,13 +2773,13 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K47" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="M47">
         <v>45</v>
@@ -2751,19 +2787,19 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D48">
-        <v>13.7462524</v>
+        <v>14.1378761</v>
       </c>
       <c r="E48">
-        <v>100.5328635</v>
+        <v>100.8255049</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -2778,13 +2814,13 @@
         <v>0</v>
       </c>
       <c r="J48" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K48" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="M48">
         <v>46</v>
@@ -2795,16 +2831,16 @@
         <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C49" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D49">
-        <v>13.7243591</v>
+        <v>13.54974685</v>
       </c>
       <c r="E49">
-        <v>100.5386589</v>
+        <v>100.2561435</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -2819,16 +2855,180 @@
         <v>0</v>
       </c>
       <c r="J49" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K49" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="M49">
         <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50">
+        <v>13.73541413</v>
+      </c>
+      <c r="E50">
+        <v>100.5877998</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50" t="s">
+        <v>89</v>
+      </c>
+      <c r="K50" t="s">
+        <v>128</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="M50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51">
+        <v>13.78766192</v>
+      </c>
+      <c r="E51">
+        <v>100.5105938</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>89</v>
+      </c>
+      <c r="K51" t="s">
+        <v>129</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="M51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52">
+        <v>13.7462524</v>
+      </c>
+      <c r="E52">
+        <v>100.5328635</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>89</v>
+      </c>
+      <c r="K52" t="s">
+        <v>130</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="M52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53">
+        <v>13.7243591</v>
+      </c>
+      <c r="E53">
+        <v>100.5386589</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>89</v>
+      </c>
+      <c r="K53" t="s">
+        <v>131</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="M53">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2878,9 +3078,13 @@
     <hyperlink ref="L44" r:id="rId43"/>
     <hyperlink ref="L45" r:id="rId44"/>
     <hyperlink ref="L46" r:id="rId45"/>
-    <hyperlink ref="L47" r:id="rId46" location="cxrecs_s"/>
-    <hyperlink ref="L48" r:id="rId47"/>
+    <hyperlink ref="L47" r:id="rId46"/>
+    <hyperlink ref="L48" r:id="rId47" location="cxrecs_s"/>
     <hyperlink ref="L49" r:id="rId48"/>
+    <hyperlink ref="L50" r:id="rId49"/>
+    <hyperlink ref="L51" r:id="rId50"/>
+    <hyperlink ref="L52" r:id="rId51"/>
+    <hyperlink ref="L53" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Recent 7 Days Alert Data 🔥
</commit_message>
<xml_diff>
--- a/dataset/xlsx/covid-tracker.xlsx
+++ b/dataset/xlsx/covid-tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="158">
   <si>
     <t>status</t>
   </si>
@@ -115,9 +115,6 @@
     <t>2020-12-17</t>
   </si>
   <si>
-    <t>2020-12-18</t>
-  </si>
-  <si>
     <t>2020-12-19</t>
   </si>
   <si>
@@ -223,54 +220,57 @@
     <t>นนทบุรี</t>
   </si>
   <si>
+    <t>แพกุ้งขนาดเล็ก บริเวณใกล้หอนาฬิกา</t>
+  </si>
+  <si>
+    <t>สำนักงานขนส่งเขตบางขุนเทียน</t>
+  </si>
+  <si>
+    <t>INC2 Tower B</t>
+  </si>
+  <si>
+    <t>ตลาดหมู่บ้านศรีทอง จ.อยุธยา</t>
+  </si>
+  <si>
+    <t xml:space="preserve">รามอินทรา </t>
+  </si>
+  <si>
+    <t>ตลาดกลางกุ้งจังหวัดสมุทรสาคร</t>
+  </si>
+  <si>
+    <t>เสรีไทย ซ.50</t>
+  </si>
+  <si>
     <t>ตลาดยายพ่วง มหาชัย</t>
   </si>
   <si>
-    <t>แพกุ้งขนาดเล็ก บริเวณใกล้หอนาฬิกา</t>
-  </si>
-  <si>
-    <t>สำนักงานขนส่งเขตบางขุนเทียน</t>
+    <t>ร้านอาหารแห่งหนึ่ง</t>
+  </si>
+  <si>
+    <t>ตลาดหนองเสือ</t>
+  </si>
+  <si>
+    <t>Lamptitude สาขาเอกมัย</t>
+  </si>
+  <si>
+    <t>กรมชลประทาน</t>
+  </si>
+  <si>
+    <t>ตลาดเจดีย์</t>
+  </si>
+  <si>
+    <t>Siam Center</t>
+  </si>
+  <si>
+    <t>อาคารกรุงเทพประกันภัย ชั้น 22</t>
+  </si>
+  <si>
+    <t>ตลาดทะเลไทย</t>
   </si>
   <si>
     <t>ตลาดหน้าสถานีรถไฟภาชี</t>
   </si>
   <si>
-    <t>INC2 Tower B</t>
-  </si>
-  <si>
-    <t>ตลาดกลางกุ้งจังหวัดสมุทรสาคร</t>
-  </si>
-  <si>
-    <t>ตลาดหมู่บ้านศรีทอง จ.อยุธยา</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รามอินทรา </t>
-  </si>
-  <si>
-    <t>เสรีไทย ซ.50</t>
-  </si>
-  <si>
-    <t>ร้านอาหารแห่งหนึ่ง</t>
-  </si>
-  <si>
-    <t>ตลาดหนองเสือ</t>
-  </si>
-  <si>
-    <t>ตลาดทะเลไทย</t>
-  </si>
-  <si>
-    <t>Lamptitude สาขาเอกมัย</t>
-  </si>
-  <si>
-    <t>กรมชลประทาน</t>
-  </si>
-  <si>
-    <t>Siam Center</t>
-  </si>
-  <si>
-    <t>อาคารกรุงเทพประกันภัย ชั้น 22</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
@@ -373,45 +373,48 @@
     <t xml:space="preserve">เคสแม่ค้ารถพุ่มพวงติดโควิด เป็นรถกระบะสีขาว ป้ายแดง ทะเบียน 8681 สมุทรปราการ </t>
   </si>
   <si>
+    <t>เคสบุคลากร สวทช. ติดโควิด-19 ได้เข้ามาต่อใบขับขี่ที่นี่วันที่ 15 ธ.ค. ตรวจพบเชื้อตอนเย็นวันที่ 17 ธ.ค.</t>
+  </si>
+  <si>
+    <t>เคสบุคลากร สวทช. ติดโควิด-19 ได้เข้ามาปฏิบัติงานที่นี่วันที่ 16-17 ธ.ค. ตรวจพบเชื้อตอนเย็นวันที่ 17 ธ.ค.</t>
+  </si>
+  <si>
+    <t>พบผู้ป่วยติดเชื้อโควิด-19 ไม่มีอาการ จำนวน 1 ราย เป็นหญิง เดินทางกลับมาจากการไปทำงานที่ร้านเสริมสวยใน จ.เชียงใหม่</t>
+  </si>
+  <si>
+    <t>พบการแพร่ระบาดของโควิดในตลาดกุ้ง และในพื้นที่ จ.สมุทรสาคร</t>
+  </si>
+  <si>
     <t>เคสเจ้าของร้านอาหารติดโควิด มีประวัติไปแพกุ้ง ตลาดยายพ่วง มหาชัย</t>
   </si>
   <si>
-    <t>เคสบุคลากร สวทช. ติดโควิด-19 ได้เข้ามาต่อใบขับขี่ที่นี่วันที่ 15 ธ.ค. ตรวจพบเชื้อตอนเย็นวันที่ 17 ธ.ค.</t>
+    <t>ขอให้ผู้ที่ไปใช้บริการร้านอาหาร ตั้งแต่วันที่ 15-20 ธ.ค. 2563 เป็นต้นมา ณ ร้านแจ่วฮ้อนตาแป๊ะบุฟเฟ่ 149 ซึ่งมี 3 สาขา สาขาที่ 1 อำเภอหนองแค สาขา 2 อำเภอแก่งคอย และสาขา 3 อำเภอเมืองสระบุรี และตลาดหนองเสือ จ.ปทุมธานี ได้สังเกตอาการตนเองเป็นเวลา 14 วัน ให้สวมหน้ากากอนามัย หรือหน้ากากผ้าตลอดเวลา หลีกเลี่ยงคลุกคลีใกล้ชิดกับผู้อื่น</t>
+  </si>
+  <si>
+    <t>เจ้าของร้านอาหารที่ติดโควิดได้ไปขายเนื้อสดที่ตลาด</t>
+  </si>
+  <si>
+    <t>พนักงาน Lamptitude ติดเชื้อหลังจากกลับจากกระบี่ และเข้ามาที่นี่ตั้งแต่วันที่ 14-22 ธ.ค.</t>
+  </si>
+  <si>
+    <t>เจ้าหน้าที่กรมชลประทานพบผู้ติดเชื้อโควิด-19 เบื้องต้น 1 ราย เป็นวิศวกร สังกัด​กองพัฒนาแหล่ง​น้ำ​ขนาดกลาง โดยได้เดินทางไปรับประทานอาหารในพื้นที่เสี่ยง จังหวัดสมุทรสาคร เมื่อวันที่ 13 ธันวาคมที่ผ่านมา</t>
+  </si>
+  <si>
+    <t>มีรายงานข่าวว่าพ่อค้าที่ติดโควิด-19 รับอาหารทะเลจากตลาดในจ.สมุทรสาครมาขายที่นี่</t>
+  </si>
+  <si>
+    <t>สยามเซ็นเตอร์' ประกาศยืนยันมี พนง.ร้านอาหารติดเชื้อโควิด-19 ขอปิดบริการพื้นที่เสี่ยง 3 วัน</t>
+  </si>
+  <si>
+    <t>บมจ.กรุงเทพประกันภัย (BKI) แจ้งว่า พบพนักงานของ บมจ.ไอโออิ กรุงเทพประกันภัย จำกัด ซึ่งเป็นบริษัทผู้เช่าในอาคารกรุงเทพประกันภัย 1 รายติดเชื้อโควิด-19 ซึ่งผู้ติดเชื้อได้ทราบผลและการยืนยันจากแพทย์ว่าติดเชื้อโควิด-19 เมื่อวันที่ 22 ธ.ค.</t>
+  </si>
+  <si>
+    <t>พบแม่ค้าอยุธยาเดินทางมาซื้ออาหารทะเลที่นี่และติดเชื่อโควิด-19</t>
   </si>
   <si>
     <t>แม่ค้าอาหารทะเล ติดเชื้อจากการเดินทางไปตลาดทะเลไทย จ.สมุทรสาคร</t>
   </si>
   <si>
-    <t>เคสบุคลากร สวทช. ติดโควิด-19 ได้เข้ามาปฏิบัติงานที่นี่วันที่ 16-17 ธ.ค. ตรวจพบเชื้อตอนเย็นวันที่ 17 ธ.ค.</t>
-  </si>
-  <si>
-    <t>พบการแพร่ระบาดของโควิดในตลาดกุ้ง และในพื้นที่ จ.สมุทรสาคร</t>
-  </si>
-  <si>
-    <t>พบผู้ป่วยติดเชื้อโควิด-19 ไม่มีอาการ จำนวน 1 ราย เป็นหญิง เดินทางกลับมาจากการไปทำงานที่ร้านเสริมสวยใน จ.เชียงใหม่</t>
-  </si>
-  <si>
-    <t>ขอให้ผู้ที่ไปใช้บริการร้านอาหาร ตั้งแต่วันที่ 15-20 ธ.ค. 2563 เป็นต้นมา ณ ร้านแจ่วฮ้อนตาแป๊ะบุฟเฟ่ 149 ซึ่งมี 3 สาขา สาขาที่ 1 อำเภอหนองแค สาขา 2 อำเภอแก่งคอย และสาขา 3 อำเภอเมืองสระบุรี และตลาดหนองเสือ จ.ปทุมธานี ได้สังเกตอาการตนเองเป็นเวลา 14 วัน ให้สวมหน้ากากอนามัย หรือหน้ากากผ้าตลอดเวลา หลีกเลี่ยงคลุกคลีใกล้ชิดกับผู้อื่น</t>
-  </si>
-  <si>
-    <t>เจ้าของร้านอาหารที่ติดโควิดได้ไปขายเนื้อสดที่ตลาด</t>
-  </si>
-  <si>
-    <t>พบแม่ค้าอยุธยาเดินทางมาซื้ออาหารทะเลที่นี่และติดเชื่อโควิด-19</t>
-  </si>
-  <si>
-    <t>พนักงาน Lamptitude ติดเชื้อหลังจากกลับจากกระบี่ และเข้ามาที่นี่ตั้งแต่วันที่ 14-22 ธ.ค.</t>
-  </si>
-  <si>
-    <t>เจ้าหน้าที่กรมชลประทานพบผู้ติดเชื้อโควิด-19 เบื้องต้น 1 ราย เป็นวิศวกร สังกัด​กองพัฒนาแหล่ง​น้ำ​ขนาดกลาง โดยได้เดินทางไปรับประทานอาหารในพื้นที่เสี่ยง จังหวัดสมุทรสาคร เมื่อวันที่ 13 ธันวาคมที่ผ่านมา</t>
-  </si>
-  <si>
-    <t>สยามเซ็นเตอร์' ประกาศยืนยันมี พนง.ร้านอาหารติดเชื้อโควิด-19 ขอปิดบริการพื้นที่เสี่ยง 3 วัน</t>
-  </si>
-  <si>
-    <t>บมจ.กรุงเทพประกันภัย (BKI) แจ้งว่า พบพนักงานของ บมจ.ไอโออิ กรุงเทพประกันภัย จำกัด ซึ่งเป็นบริษัทผู้เช่าในอาคารกรุงเทพประกันภัย 1 รายติดเชื้อโควิด-19 ซึ่งผู้ติดเชื้อได้ทราบผลและการยืนยันจากแพทย์ว่าติดเชื้อโควิด-19 เมื่อวันที่ 22 ธ.ค.</t>
-  </si>
-  <si>
     <t>https://www.facebook.com/onenews31/posts/3330353970386388</t>
   </si>
   <si>
@@ -454,34 +457,37 @@
     <t>https://www.thairath.co.th/news/local/central/1999153</t>
   </si>
   <si>
+    <t>https://www.matichon.co.th/covid19/thai-covid19/news_2492767</t>
+  </si>
+  <si>
+    <t>https://www.thaipost.net/main/detail/87367</t>
+  </si>
+  <si>
+    <t>https://www.thairath.co.th/news/local/east/1998735</t>
+  </si>
+  <si>
+    <t>https://www.thairath.co.th/news/local/central/1998711</t>
+  </si>
+  <si>
+    <t>https://www.thairath.co.th/news/local/central/1998795?cx_testId=0&amp;cx_testVariant=cx_0&amp;cx_artPos=0&amp;cx_rec_section=news&amp;cx_rec_topic=local#cxrecs_s</t>
+  </si>
+  <si>
+    <t>https://www.pptvhd36.com/news/%E0%B8%AA%E0%B8%B1%E0%B8%87%E0%B8%84%E0%B8%A1/138884</t>
+  </si>
+  <si>
+    <t>https://www.prachachat.net/economy/news-579476</t>
+  </si>
+  <si>
+    <t>https://www.khaosod.co.th/covid-19/news_5583210</t>
+  </si>
+  <si>
+    <t>https://ch3thailandnews.bectero.com/news/224324</t>
+  </si>
+  <si>
+    <t>https://www.infoquest.co.th/2020/54934</t>
+  </si>
+  <si>
     <t>https://www.thairath.co.th/news/local/central/1999848</t>
-  </si>
-  <si>
-    <t>https://www.thaipost.net/main/detail/87367</t>
-  </si>
-  <si>
-    <t>https://www.matichon.co.th/covid19/thai-covid19/news_2492767</t>
-  </si>
-  <si>
-    <t>https://www.thairath.co.th/news/local/east/1998735</t>
-  </si>
-  <si>
-    <t>https://www.thairath.co.th/news/local/central/1998711</t>
-  </si>
-  <si>
-    <t>https://www.thairath.co.th/news/local/central/1998795?cx_testId=0&amp;cx_testVariant=cx_0&amp;cx_artPos=0&amp;cx_rec_section=news&amp;cx_rec_topic=local#cxrecs_s</t>
-  </si>
-  <si>
-    <t>https://www.pptvhd36.com/news/%E0%B8%AA%E0%B8%B1%E0%B8%87%E0%B8%84%E0%B8%A1/138884</t>
-  </si>
-  <si>
-    <t>https://www.prachachat.net/economy/news-579476</t>
-  </si>
-  <si>
-    <t>https://ch3thailandnews.bectero.com/news/224324</t>
-  </si>
-  <si>
-    <t>https://www.infoquest.co.th/2020/54934</t>
   </si>
 </sst>
 </file>
@@ -852,7 +858,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -907,7 +913,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2">
         <v>12.674583</v>
@@ -934,7 +940,7 @@
         <v>90</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -948,7 +954,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3">
         <v>13.7250712</v>
@@ -975,7 +981,7 @@
         <v>91</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -989,7 +995,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4">
         <v>12.6838253</v>
@@ -1016,7 +1022,7 @@
         <v>92</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M4">
         <v>2</v>
@@ -1030,7 +1036,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5">
         <v>12.6959971</v>
@@ -1057,7 +1063,7 @@
         <v>93</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="M5">
         <v>3</v>
@@ -1071,7 +1077,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6">
         <v>12.6833042</v>
@@ -1098,7 +1104,7 @@
         <v>94</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="M6">
         <v>4</v>
@@ -1112,7 +1118,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7">
         <v>13.653942</v>
@@ -1139,7 +1145,7 @@
         <v>95</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="M7">
         <v>5</v>
@@ -1153,7 +1159,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8">
         <v>13.700916</v>
@@ -1180,7 +1186,7 @@
         <v>96</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="M8">
         <v>6</v>
@@ -1194,7 +1200,7 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9">
         <v>13.829441</v>
@@ -1221,7 +1227,7 @@
         <v>97</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="M9">
         <v>7</v>
@@ -1235,7 +1241,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10">
         <v>13.759791</v>
@@ -1262,7 +1268,7 @@
         <v>98</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="M10">
         <v>8</v>
@@ -1276,7 +1282,7 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11">
         <v>13.845817</v>
@@ -1303,7 +1309,7 @@
         <v>99</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="M11">
         <v>9</v>
@@ -1317,7 +1323,7 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12">
         <v>18.81089258</v>
@@ -1344,7 +1350,7 @@
         <v>100</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M12">
         <v>10</v>
@@ -1358,7 +1364,7 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13">
         <v>18.80951974</v>
@@ -1385,7 +1391,7 @@
         <v>101</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M13">
         <v>11</v>
@@ -1399,7 +1405,7 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14">
         <v>18.80401814</v>
@@ -1426,7 +1432,7 @@
         <v>102</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M14">
         <v>12</v>
@@ -1440,7 +1446,7 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15">
         <v>18.80732484</v>
@@ -1467,7 +1473,7 @@
         <v>103</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M15">
         <v>13</v>
@@ -1481,7 +1487,7 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16">
         <v>18.80709567</v>
@@ -1508,7 +1514,7 @@
         <v>104</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M16">
         <v>14</v>
@@ -1522,7 +1528,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17">
         <v>18.80650918</v>
@@ -1549,7 +1555,7 @@
         <v>105</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M17">
         <v>15</v>
@@ -1563,7 +1569,7 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D18">
         <v>18.80657601</v>
@@ -1590,7 +1596,7 @@
         <v>106</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M18">
         <v>16</v>
@@ -1604,7 +1610,7 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19">
         <v>18.80658294</v>
@@ -1631,7 +1637,7 @@
         <v>107</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M19">
         <v>17</v>
@@ -1645,7 +1651,7 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20">
         <v>18.80675924</v>
@@ -1672,7 +1678,7 @@
         <v>108</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M20">
         <v>18</v>
@@ -1686,7 +1692,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21">
         <v>18.80629446</v>
@@ -1713,7 +1719,7 @@
         <v>109</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M21">
         <v>19</v>
@@ -1727,7 +1733,7 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D22">
         <v>19.85327262</v>
@@ -1754,7 +1760,7 @@
         <v>110</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="M22">
         <v>20</v>
@@ -1768,7 +1774,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23">
         <v>19.90661769</v>
@@ -1795,7 +1801,7 @@
         <v>111</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="M23">
         <v>21</v>
@@ -1809,7 +1815,7 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D24">
         <v>19.6476693</v>
@@ -1836,7 +1842,7 @@
         <v>112</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="M24">
         <v>22</v>
@@ -1850,7 +1856,7 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25">
         <v>13.7238495</v>
@@ -1877,7 +1883,7 @@
         <v>113</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M25">
         <v>23</v>
@@ -1891,7 +1897,7 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26">
         <v>13.7285268</v>
@@ -1918,7 +1924,7 @@
         <v>113</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M26">
         <v>24</v>
@@ -1932,7 +1938,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27">
         <v>13.7292718</v>
@@ -1959,7 +1965,7 @@
         <v>114</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M27">
         <v>25</v>
@@ -1973,7 +1979,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28">
         <v>14.896466</v>
@@ -2000,7 +2006,7 @@
         <v>115</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="M28">
         <v>26</v>
@@ -2014,7 +2020,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D29">
         <v>13.7499881</v>
@@ -2041,7 +2047,7 @@
         <v>116</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M29">
         <v>27</v>
@@ -2055,7 +2061,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D30">
         <v>13.6910012</v>
@@ -2082,7 +2088,7 @@
         <v>116</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M30">
         <v>28</v>
@@ -2096,7 +2102,7 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D31">
         <v>13.7468252</v>
@@ -2123,7 +2129,7 @@
         <v>116</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M31">
         <v>29</v>
@@ -2137,7 +2143,7 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32">
         <v>13.7449539</v>
@@ -2164,7 +2170,7 @@
         <v>117</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M32">
         <v>30</v>
@@ -2178,7 +2184,7 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D33">
         <v>13.8205741</v>
@@ -2205,7 +2211,7 @@
         <v>118</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M33">
         <v>31</v>
@@ -2213,19 +2219,19 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D34">
-        <v>13.5455607</v>
+        <v>13.5440411</v>
       </c>
       <c r="E34">
-        <v>100.2767611</v>
+        <v>100.2752457</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -2243,10 +2249,10 @@
         <v>89</v>
       </c>
       <c r="K34" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M34">
         <v>32</v>
@@ -2254,19 +2260,19 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
         <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D35">
-        <v>13.5440411</v>
+        <v>13.6211105</v>
       </c>
       <c r="E35">
-        <v>100.2752457</v>
+        <v>100.4387341</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2284,7 +2290,7 @@
         <v>89</v>
       </c>
       <c r="K35" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>144</v>
@@ -2295,19 +2301,19 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D36">
-        <v>13.6211105</v>
+        <v>13.8330877</v>
       </c>
       <c r="E36">
-        <v>100.4387341</v>
+        <v>100.499237</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -2325,10 +2331,10 @@
         <v>89</v>
       </c>
       <c r="K36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="M36">
         <v>34</v>
@@ -2336,19 +2342,19 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D37">
-        <v>13.8330877</v>
+        <v>14.0782451</v>
       </c>
       <c r="E37">
-        <v>100.499237</v>
+        <v>100.604118</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -2366,10 +2372,10 @@
         <v>89</v>
       </c>
       <c r="K37" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M37">
         <v>35</v>
@@ -2380,22 +2386,22 @@
         <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38">
-        <v>14.45160513</v>
+        <v>14.1487352</v>
       </c>
       <c r="E38">
-        <v>100.7230585</v>
+        <v>100.6155778</v>
       </c>
       <c r="F38">
         <v>0</v>
       </c>
-      <c r="G38">
-        <v>0</v>
+      <c r="G38" t="s">
+        <v>86</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2410,7 +2416,7 @@
         <v>121</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M38">
         <v>36</v>
@@ -2418,19 +2424,19 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D39">
-        <v>14.0782451</v>
+        <v>13.8057625</v>
       </c>
       <c r="E39">
-        <v>100.604118</v>
+        <v>100.6621959</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2448,10 +2454,10 @@
         <v>89</v>
       </c>
       <c r="K39" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="M39">
         <v>37</v>
@@ -2462,10 +2468,10 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D40">
         <v>13.5579068</v>
@@ -2489,10 +2495,10 @@
         <v>89</v>
       </c>
       <c r="K40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="M40">
         <v>38</v>
@@ -2500,25 +2506,25 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B41" t="s">
         <v>34</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D41">
-        <v>14.1487352</v>
+        <v>13.7937004</v>
       </c>
       <c r="E41">
-        <v>100.6155778</v>
+        <v>100.6923144</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
-      <c r="G41" t="s">
-        <v>86</v>
+      <c r="G41">
+        <v>0</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -2530,10 +2536,10 @@
         <v>89</v>
       </c>
       <c r="K41" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M41">
         <v>39</v>
@@ -2541,19 +2547,19 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
         <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D42">
-        <v>13.8057625</v>
+        <v>13.5455607</v>
       </c>
       <c r="E42">
-        <v>100.6621959</v>
+        <v>100.2767611</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2571,7 +2577,7 @@
         <v>89</v>
       </c>
       <c r="K42" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>145</v>
@@ -2582,19 +2588,19 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D43">
-        <v>13.7937004</v>
+        <v>13.7204469</v>
       </c>
       <c r="E43">
-        <v>100.6923144</v>
+        <v>100.5004708</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -2612,10 +2618,10 @@
         <v>89</v>
       </c>
       <c r="K43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="M43">
         <v>41</v>
@@ -2623,19 +2629,19 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D44">
-        <v>13.7204469</v>
+        <v>14.3355326</v>
       </c>
       <c r="E44">
-        <v>100.5004708</v>
+        <v>100.87017</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -2653,10 +2659,10 @@
         <v>89</v>
       </c>
       <c r="K44" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M44">
         <v>42</v>
@@ -2667,16 +2673,16 @@
         <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D45">
-        <v>14.3355326</v>
+        <v>14.5786407</v>
       </c>
       <c r="E45">
-        <v>100.87017</v>
+        <v>100.9662444</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -2694,7 +2700,7 @@
         <v>89</v>
       </c>
       <c r="K45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>150</v>
@@ -2708,16 +2714,16 @@
         <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D46">
-        <v>14.5786407</v>
+        <v>14.5116599</v>
       </c>
       <c r="E46">
-        <v>100.9662444</v>
+        <v>100.9094134</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -2735,7 +2741,7 @@
         <v>89</v>
       </c>
       <c r="K46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>150</v>
@@ -2746,19 +2752,19 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D47">
-        <v>14.5116599</v>
+        <v>14.1378761</v>
       </c>
       <c r="E47">
-        <v>100.9094134</v>
+        <v>100.8255049</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -2779,7 +2785,7 @@
         <v>125</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M47">
         <v>45</v>
@@ -2787,19 +2793,19 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B48" t="s">
         <v>35</v>
       </c>
       <c r="C48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D48">
-        <v>14.1378761</v>
+        <v>13.73541413</v>
       </c>
       <c r="E48">
-        <v>100.8255049</v>
+        <v>100.5877998</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -2820,7 +2826,7 @@
         <v>126</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M48">
         <v>46</v>
@@ -2828,19 +2834,19 @@
     </row>
     <row r="49" spans="1:13">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B49" t="s">
         <v>35</v>
       </c>
       <c r="C49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D49">
-        <v>13.54974685</v>
+        <v>13.78766192</v>
       </c>
       <c r="E49">
-        <v>100.2561435</v>
+        <v>100.5105938</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -2861,7 +2867,7 @@
         <v>127</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="M49">
         <v>47</v>
@@ -2869,19 +2875,19 @@
     </row>
     <row r="50" spans="1:13">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D50">
-        <v>13.73541413</v>
+        <v>13.5951449</v>
       </c>
       <c r="E50">
-        <v>100.5877998</v>
+        <v>100.5802135</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -2902,7 +2908,7 @@
         <v>128</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="M50">
         <v>48</v>
@@ -2910,19 +2916,19 @@
     </row>
     <row r="51" spans="1:13">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B51" t="s">
         <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D51">
-        <v>13.78766192</v>
+        <v>13.7462524</v>
       </c>
       <c r="E51">
-        <v>100.5105938</v>
+        <v>100.5328635</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2943,7 +2949,7 @@
         <v>129</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="M51">
         <v>49</v>
@@ -2954,16 +2960,16 @@
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D52">
-        <v>13.7462524</v>
+        <v>13.7243591</v>
       </c>
       <c r="E52">
-        <v>100.5328635</v>
+        <v>100.5386589</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -2984,7 +2990,7 @@
         <v>130</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="M52">
         <v>50</v>
@@ -2995,16 +3001,16 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D53">
-        <v>13.7243591</v>
+        <v>13.54974685</v>
       </c>
       <c r="E53">
-        <v>100.5386589</v>
+        <v>100.2561435</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -3025,10 +3031,51 @@
         <v>131</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="M53">
         <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54">
+        <v>14.45160513</v>
+      </c>
+      <c r="E54">
+        <v>100.7230585</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54" t="s">
+        <v>89</v>
+      </c>
+      <c r="K54" t="s">
+        <v>132</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="M54">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -3078,13 +3125,14 @@
     <hyperlink ref="L44" r:id="rId43"/>
     <hyperlink ref="L45" r:id="rId44"/>
     <hyperlink ref="L46" r:id="rId45"/>
-    <hyperlink ref="L47" r:id="rId46"/>
-    <hyperlink ref="L48" r:id="rId47" location="cxrecs_s"/>
+    <hyperlink ref="L47" r:id="rId46" location="cxrecs_s"/>
+    <hyperlink ref="L48" r:id="rId47"/>
     <hyperlink ref="L49" r:id="rId48"/>
     <hyperlink ref="L50" r:id="rId49"/>
     <hyperlink ref="L51" r:id="rId50"/>
     <hyperlink ref="L52" r:id="rId51"/>
     <hyperlink ref="L53" r:id="rId52"/>
+    <hyperlink ref="L54" r:id="rId53"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>